<commit_message>
inheritance cycle detection working as expected
</commit_message>
<xml_diff>
--- a/KPL-syntax.xlsx
+++ b/KPL-syntax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolankrutonog/Desktop/workspace/KPL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolankrutonog/Desktop/workspace/KrutC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE991AA-E76F-0C46-A54C-83C829EE5EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82DA7AD-C0B3-1C43-8438-8C4BF501C9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="20280" xr2:uid="{41DCE4D7-E8CE-B94F-BDB3-476A4686E939}"/>
+    <workbookView xWindow="6360" yWindow="800" windowWidth="26600" windowHeight="20280" xr2:uid="{41DCE4D7-E8CE-B94F-BDB3-476A4686E939}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>program</t>
   </si>
@@ -80,9 +80,6 @@
     <t>ID = expr;</t>
   </si>
   <si>
-    <t>(expr;)*</t>
-  </si>
-  <si>
     <t>\(expr\)</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     </r>
   </si>
   <si>
-    <t>expr[epxr]</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -411,6 +405,15 @@
       </rPr>
       <t xml:space="preserve"> { (expr;)* };</t>
     </r>
+  </si>
+  <si>
+    <t>(stmt)*</t>
+  </si>
+  <si>
+    <t>expr[epxr_list]</t>
+  </si>
+  <si>
+    <t>while (bool1 &amp;&amp; bool2)</t>
   </si>
 </sst>
 </file>
@@ -807,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44E24BAA-1346-0144-8CB4-EC18371454E6}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="161" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -820,7 +823,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -831,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -843,10 +846,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -864,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -873,7 +876,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -882,10 +885,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -902,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -933,7 +936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
@@ -941,39 +944,39 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
@@ -981,7 +984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
@@ -989,7 +992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
@@ -1005,52 +1008,55 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>38</v>
+      <c r="F32" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
@@ -1058,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
@@ -1069,7 +1075,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.2">
@@ -1077,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
@@ -1096,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.2">
@@ -1104,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.2">
@@ -1112,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>